<commit_message>
obs 9 y 20
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/obj/Release/Package/PackageTmp/Documentos/2.2 Plantilla_Electrificacion_rural.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/obj/Release/Package/PackageTmp/Documentos/2.2 Plantilla_Electrificacion_rural.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Versión borrado de meses y fechas SOLO SE DEJO AÑOS _V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0992C41E-CADC-4C99-A642-7FC2CB515ABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89906C-9E26-401B-88DC-7D05A3DB8C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2A4336DF-036F-4896-AF99-78CB4DC7A078}"/>
   </bookViews>
@@ -618,7 +618,7 @@
   <dimension ref="A1:D312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A17" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>